<commit_message>
Additional Wetland Site Survey results provided
</commit_message>
<xml_diff>
--- a/Class 1 Wetland Info for Analysis ALL.xlsx
+++ b/Class 1 Wetland Info for Analysis ALL.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\proj\CFWI_WetlandStress\Update2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C146D52-D600-4138-BBED-10A08AA2248E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A2C7FA-C515-4C42-8A60-12441EAFB4DE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26055" windowHeight="5190" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26055" windowHeight="5190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Class 1s" sheetId="4" r:id="rId1"/>
     <sheet name="StationNameCrosswalk" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Class 1s'!$A$1:$L$62</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="203">
   <si>
     <t>Ridge</t>
   </si>
@@ -641,7 +642,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -793,7 +794,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -985,20 +986,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1129,19 +1118,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1197,7 +1173,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1233,11 +1209,8 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1250,24 +1223,6 @@
     </xf>
     <xf numFmtId="1" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="18" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1296,27 +1251,42 @@
     <xf numFmtId="1" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1363,7 +1333,16 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1911,14 +1890,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L67" sqref="L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,47 +1909,47 @@
     <col min="6" max="6" width="21.85546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="21.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="40" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="40" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="32" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="32" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="17" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1990,19 +1969,19 @@
       <c r="E2" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>67.680000000000007</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="39">
+        <v>-1.08</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" s="35">
+      <c r="I2" s="28">
         <v>-81.404506999999995</v>
       </c>
-      <c r="J2" s="35">
+      <c r="J2" s="28">
         <v>28.083625999999999</v>
       </c>
       <c r="K2" s="6" t="s">
@@ -2013,7 +1992,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="36" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2028,19 +2007,19 @@
       <c r="E3" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="14">
         <v>64.47</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="39">
+        <v>-1.05</v>
+      </c>
+      <c r="H3" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I3" s="35">
+      <c r="I3" s="28">
         <v>-81.412561999999994</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="28">
         <v>28.113903000000001</v>
       </c>
       <c r="K3" s="6" t="s">
@@ -2051,7 +2030,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="36" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2066,19 +2045,19 @@
       <c r="E4" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="14">
         <v>68.34</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="39">
+        <v>-1.05</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="H4" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I4" s="35">
+      <c r="I4" s="28">
         <v>-81.418795000000003</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="28">
         <v>28.109258000000001</v>
       </c>
       <c r="K4" s="6" t="s">
@@ -2089,7 +2068,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="36" t="s">
         <v>126</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -2104,19 +2083,19 @@
       <c r="E5" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="39">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="H5" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I5" s="36">
+      <c r="I5" s="29">
         <v>-81.392284000000004</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="30">
         <v>28.077793</v>
       </c>
       <c r="K5" s="6" t="s">
@@ -2127,7 +2106,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="36" t="s">
         <v>127</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2142,19 +2121,19 @@
       <c r="E6" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="39">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I6" s="35">
+      <c r="I6" s="28">
         <v>-81.390062</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="28">
         <v>28.082236000000002</v>
       </c>
       <c r="K6" s="6" t="s">
@@ -2165,7 +2144,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -2180,19 +2159,19 @@
       <c r="E7" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>102.63</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="39">
+        <v>-0.87</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I7" s="35">
+      <c r="I7" s="28">
         <v>-81.537111999999993</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="28">
         <v>28.446165000000001</v>
       </c>
       <c r="K7" s="6" t="s">
@@ -2202,8 +2181,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2218,19 +2197,19 @@
       <c r="E8" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="14">
         <v>53.39</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I8" s="35">
+      <c r="G8" s="14">
+        <v>-1.07</v>
+      </c>
+      <c r="H8" s="14">
+        <v>52.32</v>
+      </c>
+      <c r="I8" s="28">
         <v>-81.207312999999999</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="28">
         <v>28.645854</v>
       </c>
       <c r="K8" s="6" t="s">
@@ -2240,8 +2219,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -2256,19 +2235,19 @@
       <c r="E9" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>70.44</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I9" s="35">
+      <c r="G9" s="14">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="H9" s="14">
+        <v>69.349999999999994</v>
+      </c>
+      <c r="I9" s="28">
         <v>-81.119699999999995</v>
       </c>
-      <c r="J9" s="35">
+      <c r="J9" s="28">
         <v>28.566631999999998</v>
       </c>
       <c r="K9" s="6" t="s">
@@ -2278,8 +2257,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
         <v>78</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2294,19 +2273,19 @@
       <c r="E10" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <v>87.49</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I10" s="35">
+      <c r="G10" s="14">
+        <v>-1.04</v>
+      </c>
+      <c r="H10" s="14">
+        <v>86.45</v>
+      </c>
+      <c r="I10" s="28">
         <v>-81.363090999999997</v>
       </c>
-      <c r="J10" s="35">
+      <c r="J10" s="28">
         <v>28.696596</v>
       </c>
       <c r="K10" s="9" t="s">
@@ -2316,8 +2295,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -2332,19 +2311,19 @@
       <c r="E11" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <v>74.14</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="35">
+      <c r="G11" s="14">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="H11" s="14">
+        <v>73</v>
+      </c>
+      <c r="I11" s="28">
         <v>-81.053314</v>
       </c>
-      <c r="J11" s="35">
+      <c r="J11" s="28">
         <v>28.394303000000001</v>
       </c>
       <c r="K11" s="6" t="s">
@@ -2354,8 +2333,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -2370,19 +2349,19 @@
       <c r="E12" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="14">
         <v>105.95</v>
       </c>
-      <c r="I12" s="35">
+      <c r="I12" s="28">
         <v>-81.911111000000005</v>
       </c>
-      <c r="J12" s="35">
+      <c r="J12" s="28">
         <v>28.312611</v>
       </c>
       <c r="K12" s="6" t="s">
@@ -2392,8 +2371,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
         <v>55</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -2408,20 +2387,20 @@
       <c r="E13" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <v>72.03</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="14">
         <v>-0.8</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <f t="shared" ref="H13:H18" si="0">F13+G13</f>
         <v>71.23</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I13" s="28">
         <v>-82.378218000000004</v>
       </c>
-      <c r="J13" s="35">
+      <c r="J13" s="28">
         <v>28.304856000000001</v>
       </c>
       <c r="K13" s="6" t="s">
@@ -2431,8 +2410,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
         <v>77</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -2447,20 +2426,20 @@
       <c r="E14" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <v>70.790000000000006</v>
       </c>
-      <c r="G14" s="15">
-        <v>-0.82</v>
-      </c>
-      <c r="H14" s="15">
+      <c r="G14" s="14">
+        <v>-0.8</v>
+      </c>
+      <c r="H14" s="14">
         <f t="shared" si="0"/>
-        <v>69.970000000000013</v>
-      </c>
-      <c r="I14" s="38">
+        <v>69.990000000000009</v>
+      </c>
+      <c r="I14" s="31">
         <v>-82.393055559999993</v>
       </c>
-      <c r="J14" s="38">
+      <c r="J14" s="31">
         <v>28.27631667</v>
       </c>
       <c r="K14" s="12" t="s">
@@ -2470,8 +2449,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
         <v>59</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -2486,20 +2465,20 @@
       <c r="E15" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="14">
         <v>93.9</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="14">
         <v>-1.02</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <f t="shared" si="0"/>
         <v>92.88000000000001</v>
       </c>
-      <c r="I15" s="35">
+      <c r="I15" s="28">
         <v>-82.017889999999994</v>
       </c>
-      <c r="J15" s="35">
+      <c r="J15" s="28">
         <v>28.354863000000002</v>
       </c>
       <c r="K15" s="6" t="s">
@@ -2509,8 +2488,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
         <v>61</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -2525,20 +2504,20 @@
       <c r="E16" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="14">
         <v>98.1</v>
       </c>
-      <c r="G16" s="15">
-        <v>-0.85</v>
-      </c>
-      <c r="H16" s="15">
+      <c r="G16" s="14">
+        <v>-0.82</v>
+      </c>
+      <c r="H16" s="14">
         <f t="shared" si="0"/>
-        <v>97.25</v>
-      </c>
-      <c r="I16" s="35">
+        <v>97.28</v>
+      </c>
+      <c r="I16" s="28">
         <v>-81.971260000000001</v>
       </c>
-      <c r="J16" s="35">
+      <c r="J16" s="28">
         <v>28.394559999999998</v>
       </c>
       <c r="K16" s="6" t="s">
@@ -2548,8 +2527,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
         <v>73</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -2564,20 +2543,20 @@
       <c r="E17" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="14">
         <v>98.8</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="14">
         <v>-1</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="14">
         <f t="shared" si="0"/>
         <v>97.8</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="28">
         <v>-82.018658000000002</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="28">
         <v>28.368859</v>
       </c>
       <c r="K17" s="6" t="s">
@@ -2587,8 +2566,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
         <v>63</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -2603,20 +2582,20 @@
       <c r="E18" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <v>100.6</v>
       </c>
-      <c r="G18" s="15">
-        <v>-0.79</v>
-      </c>
-      <c r="H18" s="15">
+      <c r="G18" s="14">
+        <v>-0.78</v>
+      </c>
+      <c r="H18" s="14">
         <f t="shared" si="0"/>
-        <v>99.809999999999988</v>
-      </c>
-      <c r="I18" s="35">
+        <v>99.82</v>
+      </c>
+      <c r="I18" s="28">
         <v>-81.946754999999996</v>
       </c>
-      <c r="J18" s="35">
+      <c r="J18" s="28">
         <v>28.361409999999999</v>
       </c>
       <c r="K18" s="6" t="s">
@@ -2626,8 +2605,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+    <row r="19" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="36" t="s">
         <v>131</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -2642,19 +2621,19 @@
       <c r="E19" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="14">
         <v>100.83</v>
       </c>
-      <c r="I19" s="35">
+      <c r="I19" s="28">
         <v>-81.953699999999984</v>
       </c>
-      <c r="J19" s="35">
+      <c r="J19" s="28">
         <v>28.421799999999998</v>
       </c>
       <c r="K19" s="6" t="s">
@@ -2664,8 +2643,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+    <row r="20" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
         <v>132</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -2680,19 +2659,19 @@
       <c r="E20" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="14">
         <v>102.01</v>
       </c>
-      <c r="I20" s="35">
+      <c r="I20" s="28">
         <v>-81.931099999829641</v>
       </c>
-      <c r="J20" s="35">
+      <c r="J20" s="28">
         <v>28.391899999629889</v>
       </c>
       <c r="K20" s="6" t="s">
@@ -2702,8 +2681,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
         <v>133</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -2718,19 +2697,19 @@
       <c r="E21" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <v>98.397000000000006</v>
       </c>
-      <c r="I21" s="35">
+      <c r="I21" s="28">
         <v>-82.090599999999995</v>
       </c>
-      <c r="J21" s="35">
+      <c r="J21" s="28">
         <v>28.180400000000017</v>
       </c>
       <c r="K21" s="6" t="s">
@@ -2740,8 +2719,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+    <row r="22" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
         <v>134</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -2756,19 +2735,19 @@
       <c r="E22" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="14">
         <v>134.32</v>
       </c>
-      <c r="I22" s="35">
+      <c r="I22" s="28">
         <v>-81.902779602842955</v>
       </c>
-      <c r="J22" s="35">
+      <c r="J22" s="28">
         <v>28.170353959223743</v>
       </c>
       <c r="K22" s="6" t="s">
@@ -2778,8 +2757,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+    <row r="23" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
         <v>135</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -2794,19 +2773,19 @@
       <c r="E23" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="14">
         <v>134.16</v>
       </c>
-      <c r="I23" s="35">
+      <c r="I23" s="28">
         <v>-81.888300000000001</v>
       </c>
-      <c r="J23" s="35">
+      <c r="J23" s="28">
         <v>28.165200000000034</v>
       </c>
       <c r="K23" s="6" t="s">
@@ -2816,8 +2795,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+    <row r="24" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
         <v>136</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -2832,19 +2811,19 @@
       <c r="E24" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="14">
         <v>134.43</v>
       </c>
-      <c r="I24" s="35">
+      <c r="I24" s="28">
         <v>-81.896199999999993</v>
       </c>
-      <c r="J24" s="35">
+      <c r="J24" s="28">
         <v>28.161000000000012</v>
       </c>
       <c r="K24" s="6" t="s">
@@ -2855,7 +2834,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="36" t="s">
         <v>107</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -2867,22 +2846,22 @@
       <c r="D25" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="G25" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="H25" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="H25" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I25" s="38">
+      <c r="I25" s="31">
         <v>-81.208902350000002</v>
       </c>
-      <c r="J25" s="38">
+      <c r="J25" s="31">
         <v>28.3584259</v>
       </c>
       <c r="K25" s="11" t="s">
@@ -2892,8 +2871,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -2908,19 +2887,19 @@
       <c r="E26" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="14">
         <v>118.82</v>
       </c>
-      <c r="G26" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I26" s="35">
+      <c r="G26" s="14">
+        <v>-0.86</v>
+      </c>
+      <c r="H26" s="14">
+        <v>117.96</v>
+      </c>
+      <c r="I26" s="28">
         <v>-81.697513999999998</v>
       </c>
-      <c r="J26" s="35">
+      <c r="J26" s="28">
         <v>28.39695</v>
       </c>
       <c r="K26" s="6" t="s">
@@ -2930,8 +2909,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="36" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -2943,22 +2922,22 @@
       <c r="D27" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I27" s="35">
+      <c r="E27" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="14">
+        <v>-1.02</v>
+      </c>
+      <c r="H27" s="14">
+        <v>42.01</v>
+      </c>
+      <c r="I27" s="28">
         <v>-81.379811000000004</v>
       </c>
-      <c r="J27" s="35">
+      <c r="J27" s="28">
         <v>28.803796999999999</v>
       </c>
       <c r="K27" s="6" t="s">
@@ -2968,8 +2947,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
         <v>53</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -2984,20 +2963,20 @@
       <c r="E28" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="14">
         <v>64.95</v>
       </c>
-      <c r="G28" s="15">
-        <v>-0.88</v>
-      </c>
-      <c r="H28" s="15">
+      <c r="G28" s="14">
+        <v>-0.89</v>
+      </c>
+      <c r="H28" s="14">
         <f>F28+G28</f>
-        <v>64.070000000000007</v>
-      </c>
-      <c r="I28" s="35">
+        <v>64.06</v>
+      </c>
+      <c r="I28" s="28">
         <v>-82.394478000000007</v>
       </c>
-      <c r="J28" s="35">
+      <c r="J28" s="28">
         <v>28.286128000000001</v>
       </c>
       <c r="K28" s="6" t="s">
@@ -3007,8 +2986,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -3023,20 +3002,20 @@
       <c r="E29" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="14">
         <v>68.930000000000007</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="14">
         <v>-0.82</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="14">
         <f>F29+G29</f>
         <v>68.110000000000014</v>
       </c>
-      <c r="I29" s="35">
+      <c r="I29" s="28">
         <v>-82.391208000000006</v>
       </c>
-      <c r="J29" s="35">
+      <c r="J29" s="28">
         <v>28.290438999999999</v>
       </c>
       <c r="K29" s="6" t="s">
@@ -3046,8 +3025,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
         <v>128</v>
       </c>
       <c r="B30" s="9" t="s">
@@ -3059,33 +3038,33 @@
       <c r="D30" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E30" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I30" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="J30" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="L30" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+      <c r="E30" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" s="14">
+        <v>69.61</v>
+      </c>
+      <c r="G30" s="14">
+        <v>-1.06</v>
+      </c>
+      <c r="H30" s="14">
+        <v>68.55</v>
+      </c>
+      <c r="I30" s="28">
+        <v>-81.290839000000005</v>
+      </c>
+      <c r="J30" s="28">
+        <v>28.648638999999999</v>
+      </c>
+      <c r="K30" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="L30" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
         <v>129</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -3097,109 +3076,110 @@
       <c r="D31" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E31" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I31" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="J31" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="L31" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+      <c r="E31" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="14">
+        <v>66.959999999999994</v>
+      </c>
+      <c r="G31" s="14">
+        <v>-1.07</v>
+      </c>
+      <c r="H31" s="14">
+        <v>65.89</v>
+      </c>
+      <c r="I31" s="28">
+        <v>-81.193905999999998</v>
+      </c>
+      <c r="J31" s="28">
+        <v>28.641027999999999</v>
+      </c>
+      <c r="K31" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="L31" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="36" t="s">
         <v>130</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E32" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I32" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="J32" s="39" t="s">
-        <v>118</v>
+      <c r="C32" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H32" s="14">
+        <v>59.54</v>
+      </c>
+      <c r="I32" s="28">
+        <v>-81.113178000000005</v>
+      </c>
+      <c r="J32" s="28">
+        <v>28.526989</v>
       </c>
       <c r="K32" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L32" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="L32" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="36" t="s">
         <v>137</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="C33" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E33" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="F33" s="16" t="s">
+      <c r="E33" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="H33" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="I33" s="38">
+      <c r="I33" s="28">
         <v>-81.663399999999996</v>
       </c>
-      <c r="J33" s="38">
+      <c r="J33" s="28">
         <v>28.2422</v>
       </c>
       <c r="K33" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L33" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="L33" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="M33" s="14"/>
+    </row>
+    <row r="34" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="36" t="s">
         <v>50</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -3214,19 +3194,19 @@
       <c r="E34" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="14">
         <v>27.5</v>
       </c>
-      <c r="G34" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I34" s="35">
+      <c r="G34" s="14">
+        <v>-1.01</v>
+      </c>
+      <c r="H34" s="14">
+        <v>26.49</v>
+      </c>
+      <c r="I34" s="28">
         <v>-81.693251000000004</v>
       </c>
-      <c r="J34" s="35">
+      <c r="J34" s="28">
         <v>29.274909999999998</v>
       </c>
       <c r="K34" s="6" t="s">
@@ -3236,8 +3216,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+    <row r="35" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="5" t="s">
@@ -3252,19 +3232,19 @@
       <c r="E35" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="14">
         <v>97.42</v>
       </c>
-      <c r="G35" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I35" s="35">
+      <c r="G35" s="14">
+        <v>-0.88</v>
+      </c>
+      <c r="H35" s="14">
+        <v>96.54</v>
+      </c>
+      <c r="I35" s="28">
         <v>-81.657584999999997</v>
       </c>
-      <c r="J35" s="35">
+      <c r="J35" s="28">
         <v>28.531825000000001</v>
       </c>
       <c r="K35" s="6" t="s">
@@ -3274,8 +3254,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    <row r="36" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="36" t="s">
         <v>43</v>
       </c>
       <c r="B36" s="5" t="s">
@@ -3290,19 +3270,19 @@
       <c r="E36" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="15">
+      <c r="F36" s="14">
         <v>97.6</v>
       </c>
-      <c r="G36" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I36" s="35">
+      <c r="G36" s="14">
+        <v>-0.86</v>
+      </c>
+      <c r="H36" s="14">
+        <v>96.74</v>
+      </c>
+      <c r="I36" s="28">
         <v>-81.712211999999994</v>
       </c>
-      <c r="J36" s="35">
+      <c r="J36" s="28">
         <v>28.447998999999999</v>
       </c>
       <c r="K36" s="6" t="s">
@@ -3312,8 +3292,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+    <row r="37" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
         <v>80</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -3328,20 +3308,20 @@
       <c r="E37" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F37" s="15">
+      <c r="F37" s="14">
         <v>105.53</v>
       </c>
-      <c r="G37" s="15">
+      <c r="G37" s="14">
         <v>-0.9</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37" s="14">
         <f t="shared" ref="H37:H52" si="1">F37+G37</f>
         <v>104.63</v>
       </c>
-      <c r="I37" s="35">
+      <c r="I37" s="28">
         <v>-81.723410000000001</v>
       </c>
-      <c r="J37" s="35">
+      <c r="J37" s="28">
         <v>27.900860000000002</v>
       </c>
       <c r="K37" s="6" t="s">
@@ -3351,8 +3331,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+    <row r="38" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -3367,20 +3347,20 @@
       <c r="E38" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="14">
         <v>111.35</v>
       </c>
-      <c r="G38" s="15">
+      <c r="G38" s="14">
         <v>-0.97</v>
       </c>
-      <c r="H38" s="15">
+      <c r="H38" s="14">
         <f t="shared" si="1"/>
         <v>110.38</v>
       </c>
-      <c r="I38" s="35">
+      <c r="I38" s="28">
         <v>-81.578689999999995</v>
       </c>
-      <c r="J38" s="35">
+      <c r="J38" s="28">
         <v>27.90391</v>
       </c>
       <c r="K38" s="12" t="s">
@@ -3390,8 +3370,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+    <row r="39" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -3406,20 +3386,20 @@
       <c r="E39" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F39" s="15">
+      <c r="F39" s="14">
         <v>95.95</v>
       </c>
-      <c r="G39" s="15">
+      <c r="G39" s="14">
         <v>-0.78</v>
       </c>
-      <c r="H39" s="15">
+      <c r="H39" s="14">
         <f t="shared" si="1"/>
         <v>95.17</v>
       </c>
-      <c r="I39" s="35">
+      <c r="I39" s="28">
         <v>-81.492193</v>
       </c>
-      <c r="J39" s="35">
+      <c r="J39" s="28">
         <v>27.928229000000002</v>
       </c>
       <c r="K39" s="12" t="s">
@@ -3429,8 +3409,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+    <row r="40" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="36" t="s">
         <v>37</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -3445,20 +3425,20 @@
       <c r="E40" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="14">
         <v>92.04</v>
       </c>
-      <c r="G40" s="15">
+      <c r="G40" s="14">
         <v>-1.1499999999999999</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H40" s="14">
         <f t="shared" si="1"/>
         <v>90.89</v>
       </c>
-      <c r="I40" s="35">
+      <c r="I40" s="28">
         <v>-81.658534000000003</v>
       </c>
-      <c r="J40" s="35">
+      <c r="J40" s="28">
         <v>28.142372000000002</v>
       </c>
       <c r="K40" s="6" t="s">
@@ -3468,8 +3448,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+    <row r="41" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -3484,20 +3464,20 @@
       <c r="E41" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F41" s="15">
+      <c r="F41" s="14">
         <v>95.05</v>
       </c>
-      <c r="G41" s="15">
+      <c r="G41" s="14">
         <v>-1.42</v>
       </c>
-      <c r="H41" s="15">
+      <c r="H41" s="14">
         <f t="shared" si="1"/>
         <v>93.63</v>
       </c>
-      <c r="I41" s="35">
+      <c r="I41" s="28">
         <v>-81.332671000000005</v>
       </c>
-      <c r="J41" s="35">
+      <c r="J41" s="28">
         <v>27.234784999999999</v>
       </c>
       <c r="K41" s="6" t="s">
@@ -3507,8 +3487,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    <row r="42" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="36" t="s">
         <v>67</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -3523,20 +3503,20 @@
       <c r="E42" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F42" s="15">
+      <c r="F42" s="14">
         <v>111.49</v>
       </c>
-      <c r="G42" s="15">
+      <c r="G42" s="14">
         <v>-1.2</v>
       </c>
-      <c r="H42" s="15">
+      <c r="H42" s="14">
         <f t="shared" si="1"/>
         <v>110.28999999999999</v>
       </c>
-      <c r="I42" s="35">
+      <c r="I42" s="28">
         <v>-81.351758000000004</v>
       </c>
-      <c r="J42" s="35">
+      <c r="J42" s="28">
         <v>27.205946999999998</v>
       </c>
       <c r="K42" s="6" t="s">
@@ -3546,8 +3526,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="36" t="s">
         <v>69</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -3562,20 +3542,20 @@
       <c r="E43" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F43" s="15">
+      <c r="F43" s="14">
         <v>71.28</v>
       </c>
-      <c r="G43" s="15">
+      <c r="G43" s="14">
         <v>-1.18</v>
       </c>
-      <c r="H43" s="15">
+      <c r="H43" s="14">
         <f t="shared" si="1"/>
         <v>70.099999999999994</v>
       </c>
-      <c r="I43" s="35">
+      <c r="I43" s="28">
         <v>-81.362716000000006</v>
       </c>
-      <c r="J43" s="35">
+      <c r="J43" s="28">
         <v>27.344290000000001</v>
       </c>
       <c r="K43" s="6" t="s">
@@ -3585,8 +3565,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    <row r="44" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -3601,20 +3581,20 @@
       <c r="E44" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F44" s="15">
+      <c r="F44" s="14">
         <v>86.23</v>
       </c>
-      <c r="G44" s="15">
+      <c r="G44" s="14">
         <v>-1.06</v>
       </c>
-      <c r="H44" s="15">
+      <c r="H44" s="14">
         <f t="shared" si="1"/>
         <v>85.17</v>
       </c>
-      <c r="I44" s="35">
+      <c r="I44" s="28">
         <v>-81.512254999999996</v>
       </c>
-      <c r="J44" s="35">
+      <c r="J44" s="28">
         <v>27.793752999999999</v>
       </c>
       <c r="K44" s="6" t="s">
@@ -3624,8 +3604,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+    <row r="45" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="36" t="s">
         <v>71</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -3640,20 +3620,20 @@
       <c r="E45" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F45" s="15">
+      <c r="F45" s="14">
         <v>94.91</v>
       </c>
-      <c r="G45" s="15">
+      <c r="G45" s="14">
         <v>-1.1200000000000001</v>
       </c>
-      <c r="H45" s="15">
+      <c r="H45" s="14">
         <f t="shared" si="1"/>
         <v>93.789999999999992</v>
       </c>
-      <c r="I45" s="35">
+      <c r="I45" s="28">
         <v>-81.364219000000006</v>
       </c>
-      <c r="J45" s="35">
+      <c r="J45" s="28">
         <v>27.244505</v>
       </c>
       <c r="K45" s="6" t="s">
@@ -3663,8 +3643,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    <row r="46" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="36" t="s">
         <v>27</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -3679,20 +3659,20 @@
       <c r="E46" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F46" s="15">
+      <c r="F46" s="14">
         <v>105.95</v>
       </c>
-      <c r="G46" s="15">
+      <c r="G46" s="14">
         <v>-0.89</v>
       </c>
-      <c r="H46" s="15">
+      <c r="H46" s="14">
         <f t="shared" si="1"/>
         <v>105.06</v>
       </c>
-      <c r="I46" s="35">
+      <c r="I46" s="28">
         <v>-81.569989000000007</v>
       </c>
-      <c r="J46" s="35">
+      <c r="J46" s="28">
         <v>27.678405999999999</v>
       </c>
       <c r="K46" s="6" t="s">
@@ -3702,8 +3682,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+    <row r="47" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="36" t="s">
         <v>18</v>
       </c>
       <c r="B47" s="5" t="s">
@@ -3718,20 +3698,20 @@
       <c r="E47" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F47" s="15">
+      <c r="F47" s="14">
         <v>134.32</v>
       </c>
-      <c r="G47" s="15">
+      <c r="G47" s="14">
         <v>-1.01</v>
       </c>
-      <c r="H47" s="15">
+      <c r="H47" s="14">
         <f t="shared" si="1"/>
         <v>133.31</v>
       </c>
-      <c r="I47" s="35">
+      <c r="I47" s="28">
         <v>-81.768938000000006</v>
       </c>
-      <c r="J47" s="35">
+      <c r="J47" s="28">
         <v>28.107150000000001</v>
       </c>
       <c r="K47" s="6" t="s">
@@ -3741,8 +3721,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+    <row r="48" spans="1:13" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -3757,20 +3737,20 @@
       <c r="E48" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F48" s="15">
+      <c r="F48" s="14">
         <v>144.37</v>
       </c>
-      <c r="G48" s="15">
+      <c r="G48" s="14">
         <v>-0.85</v>
       </c>
-      <c r="H48" s="15">
+      <c r="H48" s="14">
         <f t="shared" si="1"/>
         <v>143.52000000000001</v>
       </c>
-      <c r="I48" s="35">
+      <c r="I48" s="28">
         <v>-81.699882000000002</v>
       </c>
-      <c r="J48" s="35">
+      <c r="J48" s="28">
         <v>27.843913000000001</v>
       </c>
       <c r="K48" s="12" t="s">
@@ -3780,8 +3760,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+    <row r="49" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -3796,20 +3776,20 @@
       <c r="E49" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F49" s="15">
+      <c r="F49" s="14">
         <v>133.36000000000001</v>
       </c>
-      <c r="G49" s="15">
+      <c r="G49" s="14">
         <v>-0.92500000000000004</v>
       </c>
-      <c r="H49" s="15">
+      <c r="H49" s="14">
         <f t="shared" si="1"/>
         <v>132.435</v>
       </c>
-      <c r="I49" s="35">
+      <c r="I49" s="28">
         <v>-81.691552000000001</v>
       </c>
-      <c r="J49" s="35">
+      <c r="J49" s="28">
         <v>27.833970000000001</v>
       </c>
       <c r="K49" s="6" t="s">
@@ -3819,8 +3799,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+    <row r="50" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -3835,20 +3815,20 @@
       <c r="E50" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F50" s="15">
+      <c r="F50" s="14">
         <v>102.81</v>
       </c>
-      <c r="G50" s="15">
+      <c r="G50" s="14">
         <v>-0.95</v>
       </c>
-      <c r="H50" s="15">
+      <c r="H50" s="14">
         <f t="shared" si="1"/>
         <v>101.86</v>
       </c>
-      <c r="I50" s="35">
+      <c r="I50" s="28">
         <v>-81.468410000000006</v>
       </c>
-      <c r="J50" s="35">
+      <c r="J50" s="28">
         <v>27.915700000000001</v>
       </c>
       <c r="K50" s="6" t="s">
@@ -3858,8 +3838,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+    <row r="51" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="36" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -3874,20 +3854,20 @@
       <c r="E51" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F51" s="15">
+      <c r="F51" s="14">
         <v>121.29</v>
       </c>
-      <c r="G51" s="15">
+      <c r="G51" s="14">
         <v>-1.03</v>
       </c>
-      <c r="H51" s="15">
+      <c r="H51" s="14">
         <f t="shared" si="1"/>
         <v>120.26</v>
       </c>
-      <c r="I51" s="35">
+      <c r="I51" s="28">
         <v>-81.553030000000007</v>
       </c>
-      <c r="J51" s="35">
+      <c r="J51" s="28">
         <v>27.827970000000001</v>
       </c>
       <c r="K51" s="12" t="s">
@@ -3897,8 +3877,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="20" t="s">
+    <row r="52" spans="1:12" s="1" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="36" t="s">
         <v>138</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -3913,20 +3893,20 @@
       <c r="E52" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F52" s="23">
+      <c r="F52" s="14">
         <v>120.1</v>
       </c>
-      <c r="G52" s="23">
+      <c r="G52" s="14">
         <v>-0.99099999999999999</v>
       </c>
-      <c r="H52" s="24">
+      <c r="H52" s="14">
         <f t="shared" si="1"/>
         <v>119.10899999999999</v>
       </c>
-      <c r="I52" s="38">
+      <c r="I52" s="28">
         <v>-81.578800000000001</v>
       </c>
-      <c r="J52" s="38">
+      <c r="J52" s="28">
         <v>27.6706</v>
       </c>
       <c r="K52" s="6" t="s">
@@ -3936,8 +3916,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+    <row r="53" spans="1:12" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -3952,19 +3932,19 @@
       <c r="E53" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F53" s="15">
+      <c r="F53" s="14">
         <v>69.37</v>
       </c>
-      <c r="G53" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H53" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I53" s="35">
+      <c r="G53" s="14">
+        <v>-1.02</v>
+      </c>
+      <c r="H53" s="14">
+        <v>68.349999999999994</v>
+      </c>
+      <c r="I53" s="28">
         <v>-81.360359000000003</v>
       </c>
-      <c r="J53" s="35">
+      <c r="J53" s="28">
         <v>28.810518999999999</v>
       </c>
       <c r="K53" s="6" t="s">
@@ -3974,8 +3954,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -3990,19 +3970,19 @@
       <c r="E54" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F54" s="15">
+      <c r="F54" s="14">
         <v>96.68</v>
       </c>
-      <c r="G54" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H54" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I54" s="35">
+      <c r="G54" s="14">
+        <v>-0.88</v>
+      </c>
+      <c r="H54" s="14">
+        <v>95.8</v>
+      </c>
+      <c r="I54" s="28">
         <v>-81.642740000000003</v>
       </c>
-      <c r="J54" s="35">
+      <c r="J54" s="28">
         <v>28.510179999999998</v>
       </c>
       <c r="K54" s="6" t="s">
@@ -4012,8 +3992,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="36" t="s">
         <v>39</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -4028,19 +4008,19 @@
       <c r="E55" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F55" s="15">
+      <c r="F55" s="14">
         <v>87.65</v>
       </c>
-      <c r="G55" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H55" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I55" s="35">
+      <c r="G55" s="14">
+        <v>-0.89</v>
+      </c>
+      <c r="H55" s="14">
+        <v>86.76</v>
+      </c>
+      <c r="I55" s="28">
         <v>-81.773330000000001</v>
       </c>
-      <c r="J55" s="35">
+      <c r="J55" s="28">
         <v>28.599640000000001</v>
       </c>
       <c r="K55" s="6" t="s">
@@ -4050,8 +4030,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -4066,19 +4046,19 @@
       <c r="E56" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F56" s="15">
+      <c r="F56" s="14">
         <v>90.37</v>
       </c>
-      <c r="G56" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H56" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I56" s="35">
+      <c r="G56" s="14">
+        <v>-0.879</v>
+      </c>
+      <c r="H56" s="14">
+        <v>89.49</v>
+      </c>
+      <c r="I56" s="28">
         <v>-81.841699000000006</v>
       </c>
-      <c r="J56" s="35">
+      <c r="J56" s="28">
         <v>28.644936999999999</v>
       </c>
       <c r="K56" s="6" t="s">
@@ -4088,8 +4068,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="36" t="s">
         <v>26</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -4104,19 +4084,19 @@
       <c r="E57" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F57" s="15">
+      <c r="F57" s="14">
         <v>68.81</v>
       </c>
-      <c r="G57" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H57" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I57" s="35">
+      <c r="G57" s="14">
+        <v>-0.93</v>
+      </c>
+      <c r="H57" s="14">
+        <v>67.88</v>
+      </c>
+      <c r="I57" s="28">
         <v>-81.469958000000005</v>
       </c>
-      <c r="J57" s="35">
+      <c r="J57" s="28">
         <v>28.617014000000001</v>
       </c>
       <c r="K57" s="6" t="s">
@@ -4126,8 +4106,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="36" t="s">
         <v>95</v>
       </c>
       <c r="B58" s="7" t="s">
@@ -4142,30 +4122,30 @@
       <c r="E58" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F58" s="15">
+      <c r="F58" s="14">
         <v>97.29</v>
       </c>
-      <c r="G58" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H58" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I58" s="37">
+      <c r="G58" s="34">
+        <v>-0.87</v>
+      </c>
+      <c r="H58" s="34">
+        <v>96.42</v>
+      </c>
+      <c r="I58" s="28">
         <v>-81.746949999999998</v>
       </c>
-      <c r="J58" s="37">
+      <c r="J58" s="28">
         <v>28.463460000000001</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L58" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="36" t="s">
         <v>97</v>
       </c>
       <c r="B59" s="7" t="s">
@@ -4177,22 +4157,22 @@
       <c r="D59" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E59" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F59" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="H59" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I59" s="37">
+      <c r="E59" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F59" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="G59" s="34">
+        <v>-0.91</v>
+      </c>
+      <c r="H59" s="34">
+        <v>78.53</v>
+      </c>
+      <c r="I59" s="28">
         <v>-81.511300000000006</v>
       </c>
-      <c r="J59" s="37">
+      <c r="J59" s="28">
         <v>28.597750000000001</v>
       </c>
       <c r="K59" s="8" t="s">
@@ -4202,8 +4182,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="36" t="s">
         <v>31</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -4218,20 +4198,20 @@
       <c r="E60" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F60" s="15">
+      <c r="F60" s="14">
         <v>131.80000000000001</v>
       </c>
-      <c r="G60" s="15">
+      <c r="G60" s="14">
         <v>-0.57999999999999996</v>
       </c>
-      <c r="H60" s="15">
+      <c r="H60" s="14">
         <f>F60+G60</f>
         <v>131.22</v>
       </c>
-      <c r="I60" s="35">
+      <c r="I60" s="28">
         <v>-81.686616000000001</v>
       </c>
-      <c r="J60" s="35">
+      <c r="J60" s="28">
         <v>27.841225000000001</v>
       </c>
       <c r="K60" s="11" t="s">
@@ -4241,8 +4221,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="36" t="s">
         <v>35</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -4257,20 +4237,20 @@
       <c r="E61" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F61" s="15">
+      <c r="F61" s="14">
         <v>150.28</v>
       </c>
-      <c r="G61" s="15">
+      <c r="G61" s="14">
         <v>-1.1100000000000001</v>
       </c>
-      <c r="H61" s="15">
+      <c r="H61" s="14">
         <f>F61+G61</f>
         <v>149.16999999999999</v>
       </c>
-      <c r="I61" s="35">
+      <c r="I61" s="28">
         <v>-81.717884999999995</v>
       </c>
-      <c r="J61" s="35">
+      <c r="J61" s="28">
         <v>27.853656000000001</v>
       </c>
       <c r="K61" s="6" t="s">
@@ -4280,11 +4260,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="20" t="s">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="B62" s="27" t="s">
+      <c r="B62" s="20" t="s">
         <v>164</v>
       </c>
       <c r="C62" s="7" t="s">
@@ -4296,19 +4276,19 @@
       <c r="E62" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F62" s="15" t="s">
+      <c r="F62" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G62" s="15" t="s">
+      <c r="G62" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H62" s="15">
+      <c r="H62" s="14">
         <v>129.33000000000001</v>
       </c>
-      <c r="I62" s="35">
+      <c r="I62" s="28">
         <v>-81.595411999999996</v>
       </c>
-      <c r="J62" s="35">
+      <c r="J62" s="28">
         <v>27.923136</v>
       </c>
       <c r="K62" s="6" t="s">
@@ -4320,11 +4300,18 @@
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="41" t="s">
+      <c r="E65" s="33" t="s">
         <v>200</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L62" xr:uid="{0C5C2870-94E9-409F-B61B-F6350F584855}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="TBD"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:H62">
     <sortCondition ref="D2:D62"/>
     <sortCondition ref="C2:C62"/>
@@ -4338,520 +4325,520 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982B1635-7E8A-4742-AADC-5A858784D034}">
   <dimension ref="B1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="14" style="25" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="14" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="25" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="18" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="18" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="18" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="18" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="18" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="18" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="18" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="18" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="18" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="18" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="18" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="18" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="18" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="18" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="18" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="18" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="18" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="18" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="18" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="18" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="18" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="25" t="s">
+      <c r="D32" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="18" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="18" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="D35" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="D38" s="25" t="s">
+      <c r="D38" s="18" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="D39" s="18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="D40" s="25" t="s">
+      <c r="D40" s="18" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="25" t="s">
+      <c r="D41" s="18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="25" t="s">
+      <c r="D42" s="18" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="C43" s="27" t="s">
+      <c r="C43" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="25" t="s">
+      <c r="D43" s="18" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="C44" s="27" t="s">
+      <c r="C44" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D44" s="25" t="s">
+      <c r="D44" s="18" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="C45" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="25" t="s">
+      <c r="D45" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="C46" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="25" t="s">
+      <c r="D46" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4859,186 +4846,186 @@
       <c r="B47" t="s">
         <v>155</v>
       </c>
-      <c r="C47" s="27" t="s">
+      <c r="C47" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="D47" s="25" t="s">
+      <c r="D47" s="18" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="28" t="s">
+      <c r="B48" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="C48" s="27" t="s">
+      <c r="C48" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="D48" s="25" t="s">
+      <c r="D48" s="18" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="28" t="s">
+      <c r="B49" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="18" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="28" t="s">
+      <c r="B50" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="C50" s="30" t="s">
+      <c r="C50" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="D50" s="25" t="s">
+      <c r="D50" s="18" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C51" s="27" t="s">
+      <c r="C51" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="D51" s="25" t="s">
+      <c r="D51" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="C52" s="27" t="s">
+      <c r="C52" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="25" t="s">
+      <c r="D52" s="18" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="C53" s="27" t="s">
+      <c r="C53" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D53" s="25" t="s">
+      <c r="D53" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="28" t="s">
+      <c r="B54" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="C54" s="27" t="s">
+      <c r="C54" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D54" s="25" t="s">
+      <c r="D54" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="22" t="s">
         <v>149</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D55" s="25" t="s">
+      <c r="D55" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="28" t="s">
+      <c r="B56" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C56" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="25" t="s">
+      <c r="D56" s="18" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="C57" s="27" t="s">
+      <c r="C57" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="D57" s="25" t="s">
+      <c r="D57" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="C58" s="27" t="s">
+      <c r="C58" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="D58" s="25" t="s">
+      <c r="D58" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="28" t="s">
+      <c r="B59" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="C59" s="27" t="s">
+      <c r="C59" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D59" s="25" t="s">
+      <c r="D59" s="18" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="28" t="s">
+      <c r="B60" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="C60" s="27" t="s">
+      <c r="C60" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D60" s="25" t="s">
+      <c r="D60" s="18" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="28" t="s">
+      <c r="B61" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="C61" s="27" t="s">
+      <c r="C61" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="D61" s="25" t="s">
+      <c r="D61" s="18" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="C62" s="27" t="s">
+      <c r="C62" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D62" s="25" t="s">
+      <c r="D62" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="28" t="s">
+      <c r="B63" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="C63" s="27" t="s">
+      <c r="C63" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D63" s="25" t="s">
+      <c r="D63" s="18" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>